<commit_message>
finished bunkers and introduced comparison plots
</commit_message>
<xml_diff>
--- a/input_data/parameters.xlsx
+++ b/input_data/parameters.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\transport_model_9th_edition\input_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AAF60B-9908-42E5-8DE0-3F800FF25E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-27045" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="gompertz_vehicles_per_stock" sheetId="1" r:id="rId1"/>
+    <sheet name="vehicles_per_stock_regions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +25,118 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="35">
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>lt</t>
+  </si>
+  <si>
+    <t>suv</t>
+  </si>
+  <si>
+    <t>bus</t>
+  </si>
+  <si>
+    <t>2w</t>
+  </si>
+  <si>
+    <t>lcv</t>
+  </si>
+  <si>
+    <t>ht</t>
+  </si>
+  <si>
+    <t>mt</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>high_freight</t>
+  </si>
+  <si>
+    <t>low_freight</t>
+  </si>
+  <si>
+    <t>Vehicle Type</t>
+  </si>
+  <si>
+    <t>gompertz_vehicles_per_stock</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>06_HKC</t>
+  </si>
+  <si>
+    <t>05_PRC</t>
+  </si>
+  <si>
+    <t>01_AUS</t>
+  </si>
+  <si>
+    <t>12_NZ</t>
+  </si>
+  <si>
+    <t>09_ROK</t>
+  </si>
+  <si>
+    <t>17_SIN</t>
+  </si>
+  <si>
+    <t>18_CT</t>
+  </si>
+  <si>
+    <t>03_CDA</t>
+  </si>
+  <si>
+    <t>20_USA</t>
+  </si>
+  <si>
+    <t>02_BD</t>
+  </si>
+  <si>
+    <t>04_CHL</t>
+  </si>
+  <si>
+    <t>07_INA</t>
+  </si>
+  <si>
+    <t>10_MAS</t>
+  </si>
+  <si>
+    <t>11_MEX</t>
+  </si>
+  <si>
+    <t>13_PNG</t>
+  </si>
+  <si>
+    <t>14_PE</t>
+  </si>
+  <si>
+    <t>15_RP</t>
+  </si>
+  <si>
+    <t>16_RUS</t>
+  </si>
+  <si>
+    <t>21_VN</t>
+  </si>
+  <si>
+    <t>19_THA</t>
+  </si>
+  <si>
+    <t>08_JPN</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -66,6 +183,86 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85F7FFD6-6732-B1FF-C789-A9DD57D9180D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4019550" y="711200"/>
+          <a:ext cx="3663950" cy="1435100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>gompertz_vehicles_per_stock</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> represents what each sotck represents in the modelling of stocks per capita.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +527,395 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" activeCellId="1" sqref="A17 D21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEE8984-537C-4C23-B933-1B759B47F023}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>